<commit_message>
Finished Male vs Female Chapter
</commit_message>
<xml_diff>
--- a/DataSets/02-bundeslaender.xlsx
+++ b/DataSets/02-bundeslaender.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_UNI Projects\DASC\AssignmentRepo\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AEDA46-EE49-4114-A69B-338E21DAC7DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C75647-F873-45C2-8F34-32CDC0CBD0BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deckblatt" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Hamburg</t>
   </si>
@@ -129,19 +129,19 @@
     <t>per_km2</t>
   </si>
   <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>inhabitants</t>
+  </si>
+  <si>
     <t>Bundesrepublik Deutschland</t>
-  </si>
-  <si>
-    <t>inhabitants</t>
-  </si>
-  <si>
-    <t>Hessen</t>
-  </si>
-  <si>
-    <t>Niedersachsen</t>
-  </si>
-  <si>
-    <t>Rheinland-Pfalz</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1076,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F18"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8"/>
@@ -1467,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2550D89D-2D01-4958-97D9-19B69B4BACEB}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1478,148 +1478,364 @@
     <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="B1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="30">
+        <v>15800.54</v>
+      </c>
+      <c r="C2" s="31">
         <v>2903773</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="D2" s="31">
+        <v>1422883</v>
+      </c>
+      <c r="E2" s="31">
+        <v>1480890</v>
+      </c>
+      <c r="F2" s="31">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="30">
+        <v>755.09</v>
+      </c>
+      <c r="C3" s="31">
         <v>1847253</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="D3" s="31">
+        <v>903974</v>
+      </c>
+      <c r="E3" s="31">
+        <v>943279</v>
+      </c>
+      <c r="F3" s="31">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="31">
+        <v>36</v>
+      </c>
+      <c r="B4" s="30">
+        <v>47709.8</v>
+      </c>
+      <c r="C4" s="31">
         <v>7993608</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="D4" s="31">
+        <v>3947571</v>
+      </c>
+      <c r="E4" s="31">
+        <v>4046037</v>
+      </c>
+      <c r="F4" s="31">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="30">
+        <v>419.37</v>
+      </c>
+      <c r="C5" s="31">
         <v>681202</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="D5" s="31">
+        <v>337001</v>
+      </c>
+      <c r="E5" s="31">
+        <v>344201</v>
+      </c>
+      <c r="F5" s="31">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="30">
+        <v>34112.44</v>
+      </c>
+      <c r="C6" s="31">
         <v>17947221</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="D6" s="31">
+        <v>8805974</v>
+      </c>
+      <c r="E6" s="31">
+        <v>9141247</v>
+      </c>
+      <c r="F6" s="31">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="30">
+        <v>21115.64</v>
+      </c>
+      <c r="C7" s="31">
+        <v>6288080</v>
+      </c>
+      <c r="D7" s="31">
+        <v>3105260</v>
+      </c>
+      <c r="E7" s="31">
+        <v>3182820</v>
+      </c>
+      <c r="F7" s="31">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="31">
-        <v>6288080</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="31">
+      <c r="B8" s="30">
+        <v>19858</v>
+      </c>
+      <c r="C8" s="31">
         <v>4093903</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="D8" s="31">
+        <v>2023004</v>
+      </c>
+      <c r="E8" s="31">
+        <v>2070899</v>
+      </c>
+      <c r="F8" s="31">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="30">
+        <v>35747.83</v>
+      </c>
+      <c r="C9" s="31">
         <v>11100394</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="D9" s="31">
+        <v>5516440</v>
+      </c>
+      <c r="E9" s="31">
+        <v>5583954</v>
+      </c>
+      <c r="F9" s="31">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="30">
+        <v>70541.570000000007</v>
+      </c>
+      <c r="C10" s="31">
         <v>13124737</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="D10" s="31">
+        <v>6507691</v>
+      </c>
+      <c r="E10" s="31">
+        <v>6617046</v>
+      </c>
+      <c r="F10" s="31">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="30">
+        <v>2571.11</v>
+      </c>
+      <c r="C11" s="31">
         <v>986887</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="D11" s="31">
+        <v>484419</v>
+      </c>
+      <c r="E11" s="31">
+        <v>502468</v>
+      </c>
+      <c r="F11" s="31">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="30">
+        <v>891.12</v>
+      </c>
+      <c r="C12" s="31">
         <v>3669491</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="D12" s="31">
+        <v>1804273</v>
+      </c>
+      <c r="E12" s="31">
+        <v>1865218</v>
+      </c>
+      <c r="F12" s="31">
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="30">
+        <v>29654.43</v>
+      </c>
+      <c r="C13" s="31">
         <v>2521893</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="D13" s="31">
+        <v>1243931</v>
+      </c>
+      <c r="E13" s="31">
+        <v>1277962</v>
+      </c>
+      <c r="F13" s="31">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="30">
+        <v>23295.22</v>
+      </c>
+      <c r="C14" s="31">
         <v>1608138</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="D14" s="31">
+        <v>792612</v>
+      </c>
+      <c r="E14" s="31">
+        <v>815526</v>
+      </c>
+      <c r="F14" s="31">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="30">
+        <v>18449.93</v>
+      </c>
+      <c r="C15" s="31">
         <v>4071971</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="D15" s="31">
+        <v>2006722</v>
+      </c>
+      <c r="E15" s="31">
+        <v>2065249</v>
+      </c>
+      <c r="F15" s="31">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="30">
+        <v>20456.509999999998</v>
+      </c>
+      <c r="C16" s="31">
         <v>2194782</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="D16" s="31">
+        <v>1079862</v>
+      </c>
+      <c r="E16" s="31">
+        <v>1114920</v>
+      </c>
+      <c r="F16" s="31">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="30">
+        <v>16202.35</v>
+      </c>
+      <c r="C17" s="31">
         <v>2133378</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="D17" s="31">
+        <v>1055996</v>
+      </c>
+      <c r="E17" s="31">
+        <v>1077382</v>
+      </c>
+      <c r="F17" s="31">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="31">
+        <v>39</v>
+      </c>
+      <c r="B18" s="33">
+        <v>357580.95</v>
+      </c>
+      <c r="C18" s="31">
         <v>83166711</v>
+      </c>
+      <c r="D18" s="31">
+        <v>41037613</v>
+      </c>
+      <c r="E18" s="31">
+        <v>42129098</v>
+      </c>
+      <c r="F18" s="32">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>